<commit_message>
Code Optimized and New Data in SemestreData
</commit_message>
<xml_diff>
--- a/XTECDigital-RelationalDB-RESTAPI/RelationalDB_RESTAPI/TempFolder/SemestreData.xlsx
+++ b/XTECDigital-RelationalDB-RESTAPI/RelationalDB_RESTAPI/TempFolder/SemestreData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMZ19\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21DD4EE-D7E2-40F5-AFFA-8EFC1CC4C51F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D1D5D8-07C3-4C2D-83CA-4DBCCC318E14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{59244665-B1CE-418E-B544-A3B9FAE98113}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="201">
   <si>
     <t>Alejandro</t>
   </si>
@@ -631,6 +631,12 @@
   </si>
   <si>
     <t>Marycruz A</t>
+  </si>
+  <si>
+    <t>2019S0019</t>
+  </si>
+  <si>
+    <t>Sergio</t>
   </si>
 </sst>
 </file>
@@ -1148,13 +1154,18 @@
     <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1520,17 +1531,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32830FA-09A8-42F5-8070-9C6E2C963F1A}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="M69" sqref="M69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -4324,8 +4337,45 @@
       </c>
     </row>
     <row r="69" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C69" s="3"/>
-      <c r="E69" s="3"/>
+      <c r="A69" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G69" s="1">
+        <v>2021</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1</v>
+      </c>
+      <c r="I69" s="1">
+        <v>2</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="M69" s="6" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:N92" xr:uid="{1AC9F382-46A8-44BB-BCFC-0D9676AE66AF}"/>
@@ -4333,5 +4383,6 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>